<commit_message>
final correct Excel Sheet Code
</commit_message>
<xml_diff>
--- a/src/test/java/com/TestNG/Day17_Feb_13_2024_DataProvider_ExcelSheet/ExcelData.xlsx
+++ b/src/test/java/com/TestNG/Day17_Feb_13_2024_DataProvider_ExcelSheet/ExcelData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarth\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210D78BE-FCCB-4552-9EB1-F69380E0F784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FA56BF-B496-4691-A375-DE20391DABAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginRediff" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>username</t>
   </si>
@@ -89,32 +89,14 @@
     <t>telephone</t>
   </si>
   <si>
-    <t>Selenium</t>
-  </si>
-  <si>
-    <t>Panda</t>
-  </si>
-  <si>
-    <t>confirmpassword</t>
-  </si>
-  <si>
-    <t>seleniumpanda7@gmail.com</t>
-  </si>
-  <si>
-    <t>seleniumpanda8@gmail.com</t>
-  </si>
-  <si>
-    <t>seleniumpanda9@gmail.com</t>
-  </si>
-  <si>
-    <t>seleniumpanda10@gmail.com</t>
+    <t>email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +121,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="24"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
@@ -154,34 +144,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <u/>
       <sz val="14"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="16"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -241,28 +205,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -546,53 +503,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.15625" defaultRowHeight="18.3" x14ac:dyDescent="0.7"/>
   <cols>
-    <col min="1" max="1" width="59.41796875" style="3" customWidth="1"/>
-    <col min="2" max="16384" width="93.15625" style="3"/>
+    <col min="1" max="16384" width="93.15625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.7">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.7">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.7">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.7">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.7">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -613,19 +569,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A43442-C5E7-47B8-9D77-709CB5BBA45F}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="24.05078125" customWidth="1"/>
-    <col min="2" max="2" width="18.41796875" customWidth="1"/>
-    <col min="3" max="3" width="22.3671875" customWidth="1"/>
-    <col min="4" max="4" width="29.26171875" customWidth="1"/>
-    <col min="5" max="5" width="41.47265625" customWidth="1"/>
+    <col min="1" max="1" width="36.15625" customWidth="1"/>
+    <col min="2" max="2" width="29.68359375" customWidth="1"/>
+    <col min="3" max="3" width="35.9453125" customWidth="1"/>
+    <col min="4" max="4" width="36.62890625" customWidth="1"/>
+    <col min="5" max="5" width="29.26171875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30.6" x14ac:dyDescent="1.1000000000000001">
@@ -638,166 +594,24 @@
       <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="18.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="5">
-        <v>9876543210</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="18.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="5">
-        <v>9876543210</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="18.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="5">
-        <v>9876543210</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="18.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="5">
-        <v>9876543210</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="5">
-        <v>9876543210</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="18.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="5">
-        <v>9876543210</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="18.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="5">
-        <v>9876543210</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="18.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="5">
-        <v>9876543210</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>3</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{844A62F8-93EC-439A-B2E9-C9AA057B5BB7}"/>
-    <hyperlink ref="D3:D9" r:id="rId2" display="Selenium@123" xr:uid="{4F81A660-4449-4312-9CE8-5312155AF223}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{B04CC41F-139A-46DD-9195-F055BA77A9A2}"/>
-    <hyperlink ref="E3:E9" r:id="rId4" display="Selenium@123" xr:uid="{9CB955DD-E5F5-42DE-8A40-980EDE3B6CE5}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2507C7-4AB5-4B65-9AA3-80CBD519A2BB}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -814,213 +628,61 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:2" ht="30.6" x14ac:dyDescent="1.1000000000000001">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:2" ht="30.6" x14ac:dyDescent="1.1000000000000001">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:2" ht="30.6" x14ac:dyDescent="1.1000000000000001">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:2" ht="30.6" x14ac:dyDescent="1.1000000000000001">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:2" ht="30.6" x14ac:dyDescent="1.1000000000000001">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:2" ht="30.6" x14ac:dyDescent="1.1000000000000001">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:2" ht="30.6" x14ac:dyDescent="1.1000000000000001">
+      <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="A9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="A10" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="A11" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="A12" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B13" s="10"/>
-    </row>
-    <row r="14" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B14" s="10"/>
-    </row>
-    <row r="15" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B15" s="10"/>
-    </row>
-    <row r="16" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B16" s="10"/>
-    </row>
-    <row r="17" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B17" s="10"/>
-    </row>
-    <row r="18" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B18" s="10"/>
-    </row>
-    <row r="19" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B19" s="10"/>
-    </row>
-    <row r="20" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B20" s="10"/>
-    </row>
-    <row r="21" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B21" s="10"/>
-    </row>
-    <row r="22" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B22" s="10"/>
-    </row>
-    <row r="23" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B23" s="10"/>
-    </row>
-    <row r="24" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B24" s="10"/>
-    </row>
-    <row r="25" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B25" s="10"/>
-    </row>
-    <row r="26" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B26" s="10"/>
-    </row>
-    <row r="27" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B27" s="10"/>
-    </row>
-    <row r="28" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B28" s="10"/>
-    </row>
-    <row r="29" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B29" s="10"/>
-    </row>
-    <row r="30" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B30" s="10"/>
-    </row>
-    <row r="31" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B31" s="10"/>
-    </row>
-    <row r="32" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B32" s="10"/>
-    </row>
-    <row r="33" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B33" s="10"/>
-    </row>
-    <row r="34" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B34" s="10"/>
-    </row>
-    <row r="35" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B35" s="10"/>
-    </row>
-    <row r="36" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B36" s="10"/>
-    </row>
-    <row r="37" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B37" s="10"/>
-    </row>
-    <row r="38" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B38" s="10"/>
-    </row>
-    <row r="39" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B39" s="10"/>
-    </row>
-    <row r="40" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B40" s="10"/>
-    </row>
-    <row r="41" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B41" s="10"/>
-    </row>
-    <row r="42" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B42" s="10"/>
-    </row>
-    <row r="43" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B43" s="10"/>
-    </row>
-    <row r="44" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B44" s="10"/>
-    </row>
-    <row r="45" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B45" s="10"/>
-    </row>
-    <row r="46" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B46" s="10"/>
-    </row>
-    <row r="47" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B47" s="10"/>
-    </row>
-    <row r="48" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B48" s="10"/>
-    </row>
-    <row r="49" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B49" s="10"/>
-    </row>
-    <row r="50" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B50" s="10"/>
-    </row>
-    <row r="51" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B51" s="10"/>
-    </row>
-    <row r="52" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B52" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1033,14 +695,7 @@
     <hyperlink ref="A8" r:id="rId7" xr:uid="{A87ACFD1-D6F6-496F-A359-28A659CDEAD7}"/>
     <hyperlink ref="B2" r:id="rId8" xr:uid="{BD2AA6D5-7C24-4DC0-BC1E-A82BC34EC867}"/>
     <hyperlink ref="B3:B8" r:id="rId9" display="Selenium@123" xr:uid="{D7247A02-2F0E-497E-805E-61EE56DDE543}"/>
-    <hyperlink ref="A9" r:id="rId10" xr:uid="{B283BB0D-2D2D-4D87-862B-295004EB4583}"/>
-    <hyperlink ref="B9" r:id="rId11" xr:uid="{552141CE-1B26-4AED-AB34-8A9E1B736113}"/>
-    <hyperlink ref="A10" r:id="rId12" xr:uid="{E7917784-8796-4B56-AA82-894D91314A12}"/>
-    <hyperlink ref="A11:A12" r:id="rId13" display="seleniumpanda8@gmail.com" xr:uid="{630042AC-1F36-43EA-90C0-CD706582E242}"/>
-    <hyperlink ref="A11" r:id="rId14" xr:uid="{8AB07008-A2A4-43AD-BB46-B513E7A76B68}"/>
-    <hyperlink ref="A12" r:id="rId15" xr:uid="{D6711BE8-A420-413F-836B-C57077200616}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>